<commit_message>
Se envian archivos de la carpeta Acumulado a Guia Apro2
</commit_message>
<xml_diff>
--- a/trabajos.inacap.2019/Preparacion y evaluacion de proyecto (PEP)/Guia ABpro N°2/assets/Flujo de caja.xlsx
+++ b/trabajos.inacap.2019/Preparacion y evaluacion de proyecto (PEP)/Guia ABpro N°2/assets/Flujo de caja.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DEC521-A354-400A-93B5-B5C562CA107A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED65FB8-3B99-4F13-BA64-042D1DA826C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1226,19 +1226,31 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="2" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="18" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="19" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="20" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1260,27 +1272,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="18" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="19" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="20" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="10" xfId="13" applyBorder="1" applyAlignment="1">
@@ -1317,6 +1308,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="11" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="2" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1695,8 +1695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AY55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U37" sqref="U37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1726,7 +1726,7 @@
     <col min="26" max="26" width="23.5546875" customWidth="1"/>
     <col min="27" max="27" width="12.5546875" customWidth="1"/>
     <col min="28" max="28" width="13.6640625" customWidth="1"/>
-    <col min="29" max="29" width="12" customWidth="1"/>
+    <col min="29" max="29" width="14.33203125" customWidth="1"/>
     <col min="30" max="30" width="12.6640625" customWidth="1"/>
     <col min="31" max="31" width="31.6640625" customWidth="1"/>
     <col min="32" max="32" width="24.33203125" customWidth="1"/>
@@ -1752,59 +1752,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:51" x14ac:dyDescent="0.3">
-      <c r="B2" s="136" t="s">
+      <c r="B2" s="124" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
       <c r="AF2" s="12"/>
     </row>
     <row r="3" spans="2:51" ht="21" x14ac:dyDescent="0.4">
-      <c r="B3" s="137" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="138"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="138"/>
-      <c r="J3" s="138"/>
-      <c r="K3" s="138"/>
-      <c r="L3" s="138"/>
-      <c r="M3" s="139"/>
+      <c r="B3" s="125" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="127"/>
       <c r="Q3" s="122" t="s">
         <v>79</v>
       </c>
-      <c r="R3" s="124"/>
-      <c r="S3" s="124"/>
-      <c r="T3" s="124"/>
+      <c r="R3" s="132"/>
+      <c r="S3" s="132"/>
+      <c r="T3" s="132"/>
       <c r="U3" s="123"/>
-      <c r="Y3" s="146" t="s">
+      <c r="Y3" s="143" t="s">
         <v>6</v>
       </c>
-      <c r="Z3" s="147"/>
-      <c r="AA3" s="147"/>
-      <c r="AB3" s="147"/>
-      <c r="AC3" s="148"/>
+      <c r="Z3" s="144"/>
+      <c r="AA3" s="144"/>
+      <c r="AB3" s="144"/>
+      <c r="AC3" s="145"/>
       <c r="AE3" s="122" t="s">
         <v>133</v>
       </c>
-      <c r="AF3" s="124"/>
-      <c r="AG3" s="124"/>
-      <c r="AH3" s="124"/>
-      <c r="AI3" s="124"/>
-      <c r="AJ3" s="124"/>
-      <c r="AK3" s="124"/>
-      <c r="AL3" s="124"/>
-      <c r="AM3" s="124"/>
-      <c r="AN3" s="124"/>
+      <c r="AF3" s="132"/>
+      <c r="AG3" s="132"/>
+      <c r="AH3" s="132"/>
+      <c r="AI3" s="132"/>
+      <c r="AJ3" s="132"/>
+      <c r="AK3" s="132"/>
+      <c r="AL3" s="132"/>
+      <c r="AM3" s="132"/>
+      <c r="AN3" s="132"/>
       <c r="AO3" s="123"/>
       <c r="AT3" s="116"/>
       <c r="AU3" s="116"/>
@@ -1863,13 +1863,13 @@
       <c r="U4" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="Y4" s="149" t="s">
+      <c r="Y4" s="146" t="s">
         <v>43</v>
       </c>
-      <c r="Z4" s="150"/>
-      <c r="AA4" s="150"/>
-      <c r="AB4" s="150"/>
-      <c r="AC4" s="151"/>
+      <c r="Z4" s="147"/>
+      <c r="AA4" s="147"/>
+      <c r="AB4" s="147"/>
+      <c r="AC4" s="148"/>
       <c r="AE4" s="90" t="s">
         <v>123</v>
       </c>
@@ -1908,20 +1908,20 @@
       <c r="AY4" s="87"/>
     </row>
     <row r="5" spans="2:51" x14ac:dyDescent="0.3">
-      <c r="B5" s="130" t="s">
+      <c r="B5" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="131"/>
-      <c r="D5" s="131"/>
-      <c r="E5" s="131"/>
-      <c r="F5" s="131"/>
-      <c r="G5" s="131"/>
-      <c r="H5" s="131"/>
-      <c r="I5" s="131"/>
-      <c r="J5" s="131"/>
-      <c r="K5" s="131"/>
-      <c r="L5" s="131"/>
-      <c r="M5" s="132"/>
+      <c r="C5" s="135"/>
+      <c r="D5" s="135"/>
+      <c r="E5" s="135"/>
+      <c r="F5" s="135"/>
+      <c r="G5" s="135"/>
+      <c r="H5" s="135"/>
+      <c r="I5" s="135"/>
+      <c r="J5" s="135"/>
+      <c r="K5" s="135"/>
+      <c r="L5" s="135"/>
+      <c r="M5" s="136"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="8" t="s">
         <v>7</v>
@@ -2600,20 +2600,20 @@
       </c>
     </row>
     <row r="12" spans="2:51" x14ac:dyDescent="0.3">
-      <c r="B12" s="133" t="s">
+      <c r="B12" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="134"/>
-      <c r="D12" s="134"/>
-      <c r="E12" s="134"/>
-      <c r="F12" s="134"/>
-      <c r="G12" s="134"/>
-      <c r="H12" s="134"/>
-      <c r="I12" s="134"/>
-      <c r="J12" s="134"/>
-      <c r="K12" s="134"/>
-      <c r="L12" s="134"/>
-      <c r="M12" s="135"/>
+      <c r="C12" s="138"/>
+      <c r="D12" s="138"/>
+      <c r="E12" s="138"/>
+      <c r="F12" s="138"/>
+      <c r="G12" s="138"/>
+      <c r="H12" s="138"/>
+      <c r="I12" s="138"/>
+      <c r="J12" s="138"/>
+      <c r="K12" s="138"/>
+      <c r="L12" s="138"/>
+      <c r="M12" s="139"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
@@ -2839,13 +2839,13 @@
         <f>SUM(T14:T15)</f>
         <v>247000</v>
       </c>
-      <c r="Y14" s="152" t="s">
+      <c r="Y14" s="149" t="s">
         <v>42</v>
       </c>
-      <c r="Z14" s="153"/>
-      <c r="AA14" s="153"/>
-      <c r="AB14" s="153"/>
-      <c r="AC14" s="154"/>
+      <c r="Z14" s="150"/>
+      <c r="AA14" s="150"/>
+      <c r="AB14" s="150"/>
+      <c r="AC14" s="151"/>
       <c r="AE14" s="95" t="s">
         <v>131</v>
       </c>
@@ -3591,10 +3591,10 @@
       <c r="M22" s="68">
         <v>0</v>
       </c>
-      <c r="Q22" s="129" t="s">
+      <c r="Q22" s="133" t="s">
         <v>90</v>
       </c>
-      <c r="R22" s="129"/>
+      <c r="R22" s="133"/>
       <c r="Y22" s="40" t="s">
         <v>55</v>
       </c>
@@ -3697,28 +3697,28 @@
       </c>
     </row>
     <row r="24" spans="2:41" ht="18" x14ac:dyDescent="0.35">
-      <c r="B24" s="140" t="s">
+      <c r="B24" s="128" t="s">
         <v>120</v>
       </c>
-      <c r="C24" s="141"/>
-      <c r="D24" s="141"/>
-      <c r="E24" s="141"/>
-      <c r="F24" s="141"/>
-      <c r="G24" s="141"/>
-      <c r="H24" s="141"/>
-      <c r="I24" s="141"/>
-      <c r="J24" s="141"/>
-      <c r="K24" s="141"/>
-      <c r="L24" s="141"/>
-      <c r="M24" s="142"/>
+      <c r="C24" s="129"/>
+      <c r="D24" s="129"/>
+      <c r="E24" s="129"/>
+      <c r="F24" s="129"/>
+      <c r="G24" s="129"/>
+      <c r="H24" s="129"/>
+      <c r="I24" s="129"/>
+      <c r="J24" s="129"/>
+      <c r="K24" s="129"/>
+      <c r="L24" s="129"/>
+      <c r="M24" s="130"/>
       <c r="Q24" s="122" t="s">
         <v>103</v>
       </c>
-      <c r="R24" s="124"/>
-      <c r="S24" s="124"/>
-      <c r="T24" s="124"/>
-      <c r="U24" s="124"/>
-      <c r="V24" s="124"/>
+      <c r="R24" s="132"/>
+      <c r="S24" s="132"/>
+      <c r="T24" s="132"/>
+      <c r="U24" s="132"/>
+      <c r="V24" s="132"/>
       <c r="W24" s="123"/>
       <c r="Y24" s="40" t="s">
         <v>59</v>
@@ -3931,13 +3931,13 @@
         <f>PMT($U$37,$U$33,-$R$29)</f>
         <v>114999127.70232336</v>
       </c>
-      <c r="Y26" s="143" t="s">
+      <c r="Y26" s="140" t="s">
         <v>62</v>
       </c>
-      <c r="Z26" s="144"/>
-      <c r="AA26" s="144"/>
-      <c r="AB26" s="144"/>
-      <c r="AC26" s="145"/>
+      <c r="Z26" s="141"/>
+      <c r="AA26" s="141"/>
+      <c r="AB26" s="141"/>
+      <c r="AC26" s="142"/>
     </row>
     <row r="27" spans="2:41" x14ac:dyDescent="0.3">
       <c r="B27" s="49" t="s">
@@ -4078,20 +4078,20 @@
       <c r="AI28" s="106"/>
     </row>
     <row r="29" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="B29" s="128" t="s">
+      <c r="B29" s="131" t="s">
         <v>155</v>
       </c>
-      <c r="C29" s="128"/>
-      <c r="D29" s="128"/>
-      <c r="E29" s="128"/>
-      <c r="F29" s="128"/>
-      <c r="G29" s="128"/>
-      <c r="H29" s="128"/>
-      <c r="I29" s="128"/>
-      <c r="J29" s="128"/>
-      <c r="K29" s="128"/>
-      <c r="L29" s="128"/>
-      <c r="M29" s="128"/>
+      <c r="C29" s="131"/>
+      <c r="D29" s="131"/>
+      <c r="E29" s="131"/>
+      <c r="F29" s="131"/>
+      <c r="G29" s="131"/>
+      <c r="H29" s="131"/>
+      <c r="I29" s="131"/>
+      <c r="J29" s="131"/>
+      <c r="K29" s="131"/>
+      <c r="L29" s="131"/>
+      <c r="M29" s="131"/>
       <c r="Q29" s="61" t="s">
         <v>93</v>
       </c>
@@ -4188,16 +4188,16 @@
       </c>
     </row>
     <row r="32" spans="2:41" ht="18" x14ac:dyDescent="0.35">
-      <c r="B32" s="125" t="s">
+      <c r="B32" s="152" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="126"/>
-      <c r="D32" s="126"/>
-      <c r="E32" s="126"/>
-      <c r="F32" s="126"/>
-      <c r="G32" s="126"/>
-      <c r="H32" s="126"/>
-      <c r="I32" s="127"/>
+      <c r="C32" s="153"/>
+      <c r="D32" s="153"/>
+      <c r="E32" s="153"/>
+      <c r="F32" s="153"/>
+      <c r="G32" s="153"/>
+      <c r="H32" s="153"/>
+      <c r="I32" s="154"/>
       <c r="Q32" s="122" t="s">
         <v>96</v>
       </c>
@@ -4353,7 +4353,7 @@
       <c r="B37" s="122" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="124"/>
+      <c r="C37" s="132"/>
       <c r="D37" s="123"/>
       <c r="F37" s="122" t="s">
         <v>149</v>
@@ -4549,18 +4549,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="T32:U32"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B24:M24"/>
-    <mergeCell ref="B29:M29"/>
-    <mergeCell ref="AE3:AO3"/>
-    <mergeCell ref="Q24:W24"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B12:M12"/>
     <mergeCell ref="Y26:AC26"/>
     <mergeCell ref="Y3:AC3"/>
     <mergeCell ref="Y4:AC4"/>
@@ -4570,6 +4558,18 @@
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="B32:I32"/>
     <mergeCell ref="B45:C45"/>
+    <mergeCell ref="AE3:AO3"/>
+    <mergeCell ref="Q24:W24"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="B12:M12"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="T32:U32"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B24:M24"/>
+    <mergeCell ref="B29:M29"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:M26">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">

</xml_diff>